<commit_message>
Added dictionary, that provides separate indication object for all users
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -980,7 +980,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -1046,6 +1046,70 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>3-я Кольцевая 58, кв. 23</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>543</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>334</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>01.10.2023 в 17:11:29</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>5734991862</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3-я Кольцевая 58, кв. 34</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>244</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>01.10.2023 в 20:46:23</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Alex Pol ID 128446192</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactoring callback function dictionary
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" tabRatio="600" firstSheet="2" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" tabRatio="600" firstSheet="3" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Еременко 38-1" sheetId="1" state="visible" r:id="rId1"/>
@@ -535,7 +535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -601,6 +601,38 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Зорге 70-1, кв. 21</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>12344</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>54321</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>02.10.2023 в 11:29:38</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Julia Polyanskaya ID 1165737993</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -612,7 +644,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -648,6 +680,70 @@
       <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Дата внесения</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Содружества 88, кв. 88</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>547</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>3743</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>03.10.2023 в 23:05:47</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Alex Pol ID 128446192</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Содружества 88, кв. 67</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>784</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>04.10.2023 в 22:07:10</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Alex Pol ID 128446192</t>
         </is>
       </c>
     </row>
@@ -712,7 +808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -775,6 +871,38 @@
       <c r="E2" t="inlineStr">
         <is>
           <t>&lt;built-in method now of type object at 0x00007FFDDA2D8980&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Стачки 204, кв. 236</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>344</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>344</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>03.10.2023 в 22:47:25</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Alex Pol ID 128446192</t>
         </is>
       </c>
     </row>
@@ -873,14 +1001,16 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="32.7265625" customWidth="1" min="1" max="1"/>
-    <col width="17.1796875" customWidth="1" min="2" max="5"/>
+    <col width="17.1796875" customWidth="1" min="2" max="4"/>
+    <col width="25.6328125" customWidth="1" min="5" max="5"/>
+    <col width="18.1796875" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -980,16 +1110,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="32.7265625" customWidth="1" min="1" max="1"/>
-    <col width="17.1796875" customWidth="1" min="2" max="5"/>
+    <col width="17.1796875" customWidth="1" min="2" max="4"/>
+    <col width="28.26953125" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1110,6 +1241,38 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3-я Кольцевая 58, кв. 34</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>02.10.2023 в 11:29:31</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Alex Pol ID 128446192</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added new indiciations in sample.xlsx
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -808,7 +808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -901,6 +901,38 @@
         </is>
       </c>
       <c r="F3" t="inlineStr">
+        <is>
+          <t>Alex Pol ID 128446192</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Стачки 204, кв. 30</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>453</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>19473</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>08.11.2023 в 14:58:41</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>Alex Pol ID 128446192</t>
         </is>

</xml_diff>